<commit_message>
Company address change in all excel template
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Buyback-Annexure-v1.xlsx
+++ b/application/controllers/excel-templates/Buyback-Annexure-v1.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-aws/application/controllers/excel-templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anujaggarwal/Downloads/Excel Template new/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -35,9 +35,6 @@
     <t>Blackmelon Advance Technology Co. Pvt. Ltd.</t>
   </si>
   <si>
-    <t>92C/1, LANE 7, EAST AZAD NAGAR, KRISHNA NAGAR, DELHI 110051</t>
-  </si>
-  <si>
     <t>Invoice Number: {meta:invoice_id}</t>
   </si>
   <si>
@@ -99,12 +96,15 @@
   </si>
   <si>
     <t>GST: {meta:gst_number}</t>
+  </si>
+  <si>
+    <t>A-1/7a, A BLOCK, KRISHNA NAGAR, DELHI 110051</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -408,21 +408,12 @@
   </cellStyleXfs>
   <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -434,18 +425,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -486,12 +465,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -503,22 +476,40 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -526,6 +517,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -537,6 +537,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -808,211 +811,211 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:G15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="4"/>
-    <col min="3" max="3" width="22.1640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="4"/>
-    <col min="5" max="5" width="20.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="36.83203125" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="14.5" style="4"/>
+    <col min="1" max="1" width="3.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="2"/>
+    <col min="3" max="3" width="22.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="2"/>
+    <col min="5" max="5" width="20.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="36.83203125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="3"/>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3"/>
-      <c r="B4" s="38" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="37"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="19" t="s">
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1"/>
+      <c r="B7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
-      <c r="B7" s="36" t="s">
+      <c r="C7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="19" t="s">
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="17"/>
-    </row>
-    <row r="8" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="37" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="19" t="s">
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="19" t="s">
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+      <c r="A11" s="1"/>
+      <c r="B11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="24"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="24"/>
-    </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.15">
-      <c r="A11" s="3"/>
-      <c r="B11" s="27" t="s">
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="1"/>
+      <c r="B12" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="28"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="3"/>
-      <c r="B12" s="29" t="s">
+      <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="G12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="30" t="s">
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="1"/>
+      <c r="B13" s="22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
-      <c r="B13" s="31" t="s">
+      <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="F13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="G13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="32" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="35"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="40"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>